<commit_message>
include download button for excel
</commit_message>
<xml_diff>
--- a/extracted_tables.xlsx
+++ b/extracted_tables.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_2ce14a3c_6" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_023cf8a7_11" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_52166d9a_11" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_c4f900c3_11" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_2c9cf0c1_11" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_c37fd4ca_12" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_9107e2cf_13" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_a279fd4c_13" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_f3ac1cfe_6" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_a38c5d5c_11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_f6dd28ed_11" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_617355eb_11" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_42baba9f_11" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_1122d327_12" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_9ccab279_13" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Unnamed_Table_20e3b24b_13" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,7 +461,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Unnamed_Table_2ce14a3c_6</t>
+          <t>Unnamed_Table_f3ac1cfe_6</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -476,12 +476,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Unnamed_Table_023cf8a7_11</t>
+          <t>Unnamed_Table_a38c5d5c_11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Model Performance by Language and License</t>
+          <t>OSS vs Proprietary Scores by Language Model</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -491,12 +491,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Unnamed_Table_52166d9a_11</t>
+          <t>Unnamed_Table_f6dd28ed_11</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OSS vs Proprietary Model Performance</t>
+          <t>Language Model Performance by License Category</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -506,12 +506,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Unnamed_Table_c4f900c3_11</t>
+          <t>Unnamed_Table_617355eb_11</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C# Language Model Performance Comparison</t>
+          <t>C# Code Generation Metric Comparison</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -521,12 +521,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Unnamed_Table_2c9cf0c1_11</t>
+          <t>Unnamed_Table_42baba9f_11</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Code Generation Quality Metrics by Model and BM25</t>
+          <t>C Sharp Code Generation Metrics Comparison</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -536,7 +536,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Unnamed_Table_c37fd4ca_12</t>
+          <t>Unnamed_Table_1122d327_12</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -551,12 +551,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Unnamed_Table_9107e2cf_13</t>
+          <t>Unnamed_Table_9ccab279_13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BLEU Scores for C Sharp Code Davinci 002 by Shot Source</t>
+          <t>C Sharp Code Davinci 002 BLEU Scores by Shot Source</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -566,12 +566,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Unnamed_Table_a279fd4c_13</t>
+          <t>Unnamed_Table_20e3b24b_13</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Code Token Accuracy by Language Model and Source</t>
+          <t>LLM Accuracy on Identifiers and Non identifiers</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>p-value</t>
+          <t>Category-p-value</t>
         </is>
       </c>
     </row>
@@ -3213,7 +3213,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Langauge</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">

</xml_diff>